<commit_message>
add image test 3, Ep and Cp
</commit_message>
<xml_diff>
--- a/project/fractal-parallel-tasks/test-plan.xlsx
+++ b/project/fractal-parallel-tasks/test-plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>#</t>
   </si>
@@ -346,12 +346,30 @@
   <si>
     <t>Fri May 22 15:36:13 EEST 2020</t>
   </si>
+  <si>
+    <t>image-huge</t>
+  </si>
+  <si>
+    <t>Mon May 25 19:02:11 EEST 2020</t>
+  </si>
+  <si>
+    <t>imageSize : 1920x1440</t>
+  </si>
+  <si>
+    <t>imageSize : 1280x960</t>
+  </si>
+  <si>
+    <t>imageSize : 640x480</t>
+  </si>
+  <si>
+    <t>Cp = p*Tp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +464,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -461,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -484,11 +510,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -516,9 +551,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -530,6 +562,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,6 +615,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>up image size</a:t>
+            </a:r>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -796,6 +910,68 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Sp(3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$33:$L$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.930931288721931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.82540057204743</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3633054311855171</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0982892770649766</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9249433106575964</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.359189351782224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.182441756636091</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.250939235543941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.415445293859863</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.760513435221256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -805,16 +981,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="534734688"/>
-        <c:axId val="534736320"/>
+        <c:axId val="1193285664"/>
+        <c:axId val="1193286208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="534734688"/>
+        <c:axId val="1193285664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numbe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>r of threads</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -852,7 +1089,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534736320"/>
+        <c:crossAx val="1193286208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -860,7 +1097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="534736320"/>
+        <c:axId val="1193286208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,6 +1117,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -911,7 +1205,1332 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534734688"/>
+        <c:crossAx val="1193285664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="bg-BG"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="bg-BG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Efficiency image size</a:t>
+            </a:r>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ep(1)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$7:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94314181543877296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87453369083702492</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82174937013911709</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77690037282518642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75527309338031712</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71814570170400149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65586203881797522</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62577160493827155</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58513708513708507</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56045946955547254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ep(2)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$20:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95637127672722777</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93578425444431013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90257486950689636</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86934052353668123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86876710406287272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78734228734228739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72839375433889886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70332666787856757</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.62005068261265861</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51211118464592986</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ep(3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$33:$M$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96546564436096549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9563501430118575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89388423853091947</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88728615963312207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89249433106575959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86326577931518533</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7987458397597208</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70318370222149629</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.74530251632554789</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68802567176106277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1466140288"/>
+        <c:axId val="1466150080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1466140288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of thread</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466150080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1466150080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466140288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="bg-BG"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="bg-BG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cost</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> image size</a:t>
+            </a:r>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cp(1)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$7:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>30007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31816</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34312</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38624</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45752</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47952</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53540</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cp(2)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$20:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>123808</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>129456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137172</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>142416</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142510</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>157248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>169974</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>176032</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>199674</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>241760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cp(3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$33:$N$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>275513</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>285368</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>288088</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>308220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>310512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>308700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>319152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344932</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>391808</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>369666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400440</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1466137024"/>
+        <c:axId val="1466139744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1466137024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numbe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>r of threads</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466139744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1466139744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cost</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="bg-BG"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466137024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1032,6 +2651,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1548,20 +3247,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>192157</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>168965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>496957</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1575,6 +4306,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>188259</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>13446</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>197222</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>129989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>510987</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>4483</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграма 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1846,15 +4637,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:M30"/>
+  <dimension ref="A5:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="5.21875" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.109375" style="3" customWidth="1"/>
@@ -1862,10 +4653,10 @@
     <col min="7" max="10" width="6.77734375" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="13" max="14" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1878,10 +4669,11 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1915,341 +4707,392 @@
       <c r="M6" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="N6" s="20" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="15">
         <v>1</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>30250</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>30751</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>30007</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>30526</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <v>31256</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <f>MIN(F7:J7)</f>
         <v>30007</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>1</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>1</v>
       </c>
+      <c r="N7" s="21">
+        <f>D7*K7</f>
+        <v>30007</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="9">
         <v>2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="15">
         <v>2</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="15">
+      <c r="E8" s="10"/>
+      <c r="F8" s="14">
         <v>15908</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="13">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12">
         <f t="shared" ref="K8:K17" si="0">MIN(F8:J8)</f>
         <v>15908</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <f>$K$7/K8</f>
         <v>1.8862836308775459</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <f>L8/D8</f>
         <v>0.94314181543877296</v>
       </c>
+      <c r="N8" s="21">
+        <f t="shared" ref="N8:N17" si="1">D8*K8</f>
+        <v>31816</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="15">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="15">
+      <c r="E9" s="10"/>
+      <c r="F9" s="14">
         <v>8578</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="13">
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12">
         <f t="shared" si="0"/>
         <v>8578</v>
       </c>
-      <c r="L9" s="13">
-        <f t="shared" ref="L9:L17" si="1">$K$7/K9</f>
+      <c r="L9" s="12">
+        <f>$K$7/K9</f>
         <v>3.4981347633480997</v>
       </c>
-      <c r="M9" s="13">
-        <f t="shared" ref="M9:M17" si="2">L9/D9</f>
+      <c r="M9" s="12">
+        <f>L9/D9</f>
         <v>0.87453369083702492</v>
       </c>
+      <c r="N9" s="21">
+        <f t="shared" si="1"/>
+        <v>34312</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="9">
         <v>4</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="15">
         <v>6</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="15">
+      <c r="E10" s="10"/>
+      <c r="F10" s="14">
         <v>6086</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13">
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="12">
         <f t="shared" si="0"/>
         <v>6086</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="12">
+        <f>$K$7/K10</f>
+        <v>4.9304962208347023</v>
+      </c>
+      <c r="M10" s="12">
+        <f>L10/D10</f>
+        <v>0.82174937013911709</v>
+      </c>
+      <c r="N10" s="21">
         <f t="shared" si="1"/>
-        <v>4.9304962208347023</v>
-      </c>
-      <c r="M10" s="13">
-        <f t="shared" si="2"/>
-        <v>0.82174937013911709</v>
+        <v>36516</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="9">
         <v>5</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="15">
         <v>8</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="15">
+      <c r="E11" s="10"/>
+      <c r="F11" s="14">
         <v>4828</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="13">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="12">
         <f t="shared" si="0"/>
         <v>4828</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="12">
+        <f>$K$7/K11</f>
+        <v>6.2152029826014914</v>
+      </c>
+      <c r="M11" s="12">
+        <f>L11/D11</f>
+        <v>0.77690037282518642</v>
+      </c>
+      <c r="N11" s="21">
         <f t="shared" si="1"/>
-        <v>6.2152029826014914</v>
-      </c>
-      <c r="M11" s="13">
-        <f t="shared" si="2"/>
-        <v>0.77690037282518642</v>
+        <v>38624</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="9">
         <v>6</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="15">
         <v>10</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="15">
+      <c r="E12" s="10"/>
+      <c r="F12" s="14">
         <v>3973</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12">
         <f t="shared" si="0"/>
         <v>3973</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="12">
+        <f>$K$7/K12</f>
+        <v>7.5527309338031712</v>
+      </c>
+      <c r="M12" s="12">
+        <f>L12/D12</f>
+        <v>0.75527309338031712</v>
+      </c>
+      <c r="N12" s="21">
         <f t="shared" si="1"/>
-        <v>7.5527309338031712</v>
-      </c>
-      <c r="M12" s="13">
-        <f t="shared" si="2"/>
-        <v>0.75527309338031712</v>
+        <v>39730</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="9">
         <v>7</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="15">
         <v>12</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="15">
+      <c r="E13" s="10"/>
+      <c r="F13" s="14">
         <v>3482</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12">
         <f t="shared" si="0"/>
         <v>3482</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="12">
+        <f>$K$7/K13</f>
+        <v>8.6177484204480184</v>
+      </c>
+      <c r="M13" s="12">
+        <f>L13/D13</f>
+        <v>0.71814570170400149</v>
+      </c>
+      <c r="N13" s="21">
         <f t="shared" si="1"/>
-        <v>8.6177484204480184</v>
-      </c>
-      <c r="M13" s="13">
-        <f t="shared" si="2"/>
-        <v>0.71814570170400149</v>
+        <v>41784</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="9">
         <v>8</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="15">
         <v>14</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="15">
+      <c r="E14" s="10"/>
+      <c r="F14" s="14">
         <v>3268</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12">
         <f t="shared" si="0"/>
         <v>3268</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="12">
+        <f>$K$7/K14</f>
+        <v>9.1820685434516527</v>
+      </c>
+      <c r="M14" s="12">
+        <f>L14/D14</f>
+        <v>0.65586203881797522</v>
+      </c>
+      <c r="N14" s="21">
         <f t="shared" si="1"/>
-        <v>9.1820685434516527</v>
-      </c>
-      <c r="M14" s="13">
-        <f t="shared" si="2"/>
-        <v>0.65586203881797522</v>
+        <v>45752</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" s="9">
         <v>9</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="15">
         <v>16</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14">
+      <c r="E15" s="11"/>
+      <c r="F15" s="13">
         <v>2997</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="13">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="12">
         <f t="shared" si="0"/>
         <v>2997</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="12">
+        <f>$K$7/K15</f>
+        <v>10.012345679012345</v>
+      </c>
+      <c r="M15" s="12">
+        <f>L15/D15</f>
+        <v>0.62577160493827155</v>
+      </c>
+      <c r="N15" s="21">
         <f t="shared" si="1"/>
-        <v>10.012345679012345</v>
-      </c>
-      <c r="M15" s="13">
-        <f t="shared" si="2"/>
-        <v>0.62577160493827155</v>
+        <v>47952</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C16" s="9">
         <v>10</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="15">
         <v>18</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="14">
+      <c r="E16" s="11"/>
+      <c r="F16" s="13">
         <v>2849</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="13">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="12">
         <f t="shared" si="0"/>
         <v>2849</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="12">
+        <f>$K$7/K16</f>
+        <v>10.532467532467532</v>
+      </c>
+      <c r="M16" s="12">
+        <f>L16/D16</f>
+        <v>0.58513708513708507</v>
+      </c>
+      <c r="N16" s="21">
         <f t="shared" si="1"/>
-        <v>10.532467532467532</v>
-      </c>
-      <c r="M16" s="13">
-        <f t="shared" si="2"/>
-        <v>0.58513708513708507</v>
+        <v>51282</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C17" s="9">
         <v>11</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="15">
         <v>20</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="14">
+      <c r="E17" s="11"/>
+      <c r="F17" s="13">
         <v>2677</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12">
         <f t="shared" si="0"/>
         <v>2677</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="12">
+        <f>$K$7/K17</f>
+        <v>11.209189391109451</v>
+      </c>
+      <c r="M17" s="12">
+        <f>L17/D17</f>
+        <v>0.56045946955547254</v>
+      </c>
+      <c r="N17" s="21">
         <f t="shared" si="1"/>
-        <v>11.209189391109451</v>
-      </c>
-      <c r="M17" s="13">
-        <f t="shared" si="2"/>
-        <v>0.56045946955547254</v>
+        <v>53540</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
+      <c r="B19" s="19"/>
       <c r="C19" s="5" t="s">
         <v>0</v>
       </c>
@@ -2283,327 +5126,796 @@
       <c r="M19" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="N19" s="20" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="15">
         <v>1</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>2</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <v>123808</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12">
         <f>MIN(F20:J20)</f>
         <v>123808</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="12">
         <v>1</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="12">
         <v>1</v>
       </c>
+      <c r="N20" s="21">
+        <f>D20*K20</f>
+        <v>123808</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="17"/>
       <c r="C21" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="15">
         <v>2</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="15">
+      <c r="E21" s="10"/>
+      <c r="F21" s="14">
         <v>64728</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13">
-        <f t="shared" ref="K21:K30" si="3">MIN(F21:J21)</f>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12">
+        <f t="shared" ref="K21:K30" si="2">MIN(F21:J21)</f>
         <v>64728</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="12">
         <f>$K$20/K21</f>
         <v>1.9127425534544555</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="12">
         <f>L21/D21</f>
         <v>0.95637127672722777</v>
       </c>
+      <c r="N21" s="21">
+        <f t="shared" ref="N21:N30" si="3">D21*K21</f>
+        <v>129456</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="9">
         <v>3</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="15">
         <v>4</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="15">
+      <c r="E22" s="10"/>
+      <c r="F22" s="14">
         <v>33076</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13">
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12">
+        <f t="shared" si="2"/>
+        <v>33076</v>
+      </c>
+      <c r="L22" s="12">
+        <f>$K$20/K22</f>
+        <v>3.7431370177772405</v>
+      </c>
+      <c r="M22" s="12">
+        <f>L22/D22</f>
+        <v>0.93578425444431013</v>
+      </c>
+      <c r="N22" s="21">
         <f t="shared" si="3"/>
-        <v>33076</v>
-      </c>
-      <c r="L22" s="13">
-        <f t="shared" ref="L22:L30" si="4">$K$20/K22</f>
-        <v>3.7431370177772405</v>
-      </c>
-      <c r="M22" s="13">
-        <f t="shared" ref="M22:M30" si="5">L22/D22</f>
-        <v>0.93578425444431013</v>
+        <v>132304</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="9">
         <v>4</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="15">
         <v>6</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="15">
+      <c r="E23" s="10"/>
+      <c r="F23" s="14">
         <v>22862</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13">
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="12">
+        <f t="shared" si="2"/>
+        <v>22862</v>
+      </c>
+      <c r="L23" s="12">
+        <f>$K$20/K23</f>
+        <v>5.4154492170413784</v>
+      </c>
+      <c r="M23" s="12">
+        <f>L23/D23</f>
+        <v>0.90257486950689636</v>
+      </c>
+      <c r="N23" s="21">
         <f t="shared" si="3"/>
-        <v>22862</v>
-      </c>
-      <c r="L23" s="13">
-        <f t="shared" si="4"/>
-        <v>5.4154492170413784</v>
-      </c>
-      <c r="M23" s="13">
-        <f t="shared" si="5"/>
-        <v>0.90257486950689636</v>
+        <v>137172</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="9">
         <v>5</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="15">
         <v>8</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="15">
+      <c r="E24" s="10"/>
+      <c r="F24" s="14">
         <v>17802</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12">
+        <f t="shared" si="2"/>
+        <v>17802</v>
+      </c>
+      <c r="L24" s="12">
+        <f>$K$20/K24</f>
+        <v>6.9547241882934498</v>
+      </c>
+      <c r="M24" s="12">
+        <f>L24/D24</f>
+        <v>0.86934052353668123</v>
+      </c>
+      <c r="N24" s="21">
         <f t="shared" si="3"/>
-        <v>17802</v>
-      </c>
-      <c r="L24" s="13">
-        <f t="shared" si="4"/>
-        <v>6.9547241882934498</v>
-      </c>
-      <c r="M24" s="13">
-        <f t="shared" si="5"/>
-        <v>0.86934052353668123</v>
+        <v>142416</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="9">
         <v>6</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="15">
         <v>10</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="15">
+      <c r="E25" s="10"/>
+      <c r="F25" s="14">
         <v>14251</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13">
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12">
+        <f t="shared" si="2"/>
+        <v>14251</v>
+      </c>
+      <c r="L25" s="12">
+        <f>$K$20/K25</f>
+        <v>8.687671040628727</v>
+      </c>
+      <c r="M25" s="12">
+        <f>L25/D25</f>
+        <v>0.86876710406287272</v>
+      </c>
+      <c r="N25" s="21">
         <f t="shared" si="3"/>
-        <v>14251</v>
-      </c>
-      <c r="L25" s="13">
-        <f t="shared" si="4"/>
-        <v>8.687671040628727</v>
-      </c>
-      <c r="M25" s="13">
-        <f t="shared" si="5"/>
-        <v>0.86876710406287272</v>
+        <v>142510</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="9">
         <v>7</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="15">
         <v>12</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="15">
+      <c r="E26" s="10"/>
+      <c r="F26" s="14">
         <v>13104</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="13">
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="12">
+        <f t="shared" si="2"/>
+        <v>13104</v>
+      </c>
+      <c r="L26" s="12">
+        <f>$K$20/K26</f>
+        <v>9.4481074481074483</v>
+      </c>
+      <c r="M26" s="12">
+        <f>L26/D26</f>
+        <v>0.78734228734228739</v>
+      </c>
+      <c r="N26" s="21">
         <f t="shared" si="3"/>
-        <v>13104</v>
-      </c>
-      <c r="L26" s="13">
-        <f t="shared" si="4"/>
-        <v>9.4481074481074483</v>
-      </c>
-      <c r="M26" s="13">
-        <f t="shared" si="5"/>
-        <v>0.78734228734228739</v>
+        <v>157248</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="9">
         <v>8</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="15">
         <v>14</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="15">
+      <c r="E27" s="10"/>
+      <c r="F27" s="14">
         <v>12141</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="13">
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="12">
+        <f t="shared" si="2"/>
+        <v>12141</v>
+      </c>
+      <c r="L27" s="12">
+        <f>$K$20/K27</f>
+        <v>10.197512560744585</v>
+      </c>
+      <c r="M27" s="12">
+        <f>L27/D27</f>
+        <v>0.72839375433889886</v>
+      </c>
+      <c r="N27" s="21">
         <f t="shared" si="3"/>
-        <v>12141</v>
-      </c>
-      <c r="L27" s="13">
-        <f t="shared" si="4"/>
-        <v>10.197512560744585</v>
-      </c>
-      <c r="M27" s="13">
-        <f t="shared" si="5"/>
-        <v>0.72839375433889886</v>
+        <v>169974</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C28" s="9">
         <v>9</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="15">
         <v>16</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="14">
+      <c r="E28" s="11"/>
+      <c r="F28" s="13">
         <v>11002</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="13">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="12">
+        <f t="shared" si="2"/>
+        <v>11002</v>
+      </c>
+      <c r="L28" s="12">
+        <f>$K$20/K28</f>
+        <v>11.253226686057081</v>
+      </c>
+      <c r="M28" s="12">
+        <f>L28/D28</f>
+        <v>0.70332666787856757</v>
+      </c>
+      <c r="N28" s="21">
         <f t="shared" si="3"/>
-        <v>11002</v>
-      </c>
-      <c r="L28" s="13">
-        <f t="shared" si="4"/>
-        <v>11.253226686057081</v>
-      </c>
-      <c r="M28" s="13">
-        <f t="shared" si="5"/>
-        <v>0.70332666787856757</v>
+        <v>176032</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C29" s="9">
         <v>10</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="15">
         <v>18</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="14">
+      <c r="E29" s="11"/>
+      <c r="F29" s="13">
         <v>11093</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="13">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="12">
+        <f t="shared" si="2"/>
+        <v>11093</v>
+      </c>
+      <c r="L29" s="12">
+        <f>$K$20/K29</f>
+        <v>11.160912287027855</v>
+      </c>
+      <c r="M29" s="12">
+        <f>L29/D29</f>
+        <v>0.62005068261265861</v>
+      </c>
+      <c r="N29" s="21">
         <f t="shared" si="3"/>
-        <v>11093</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="4"/>
-        <v>11.160912287027855</v>
-      </c>
-      <c r="M29" s="13">
-        <f t="shared" si="5"/>
-        <v>0.62005068261265861</v>
+        <v>199674</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C30" s="9">
         <v>11</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="15">
         <v>20</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="14">
+      <c r="E30" s="11"/>
+      <c r="F30" s="13">
         <v>12088</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="13">
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="12">
+        <f t="shared" si="2"/>
+        <v>12088</v>
+      </c>
+      <c r="L30" s="12">
+        <f>$K$20/K30</f>
+        <v>10.242223692918596</v>
+      </c>
+      <c r="M30" s="12">
+        <f>L30/D30</f>
+        <v>0.51211118464592986</v>
+      </c>
+      <c r="N30" s="21">
         <f t="shared" si="3"/>
-        <v>12088</v>
-      </c>
-      <c r="L30" s="13">
+        <v>241760</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="15">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10">
+        <v>2</v>
+      </c>
+      <c r="F33" s="14">
+        <v>275513</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="12">
+        <f>MIN(F33:J33)</f>
+        <v>275513</v>
+      </c>
+      <c r="L33" s="12">
+        <v>1</v>
+      </c>
+      <c r="M33" s="12">
+        <v>1</v>
+      </c>
+      <c r="N33" s="21">
+        <f>D33*K33</f>
+        <v>275513</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="9">
+        <v>2</v>
+      </c>
+      <c r="D34" s="15">
+        <v>2</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="14">
+        <v>142684</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="12">
+        <f t="shared" ref="K34:K43" si="4">MIN(F34:J34)</f>
+        <v>142684</v>
+      </c>
+      <c r="L34" s="12">
+        <f>$K$33/K34</f>
+        <v>1.930931288721931</v>
+      </c>
+      <c r="M34" s="12">
+        <f>L34/D34</f>
+        <v>0.96546564436096549</v>
+      </c>
+      <c r="N34" s="21">
+        <f t="shared" ref="N34:N43" si="5">D34*K34</f>
+        <v>285368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="9">
+        <v>3</v>
+      </c>
+      <c r="D35" s="15">
+        <v>4</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="14">
+        <v>72022</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="12">
         <f t="shared" si="4"/>
-        <v>10.242223692918596</v>
-      </c>
-      <c r="M30" s="13">
+        <v>72022</v>
+      </c>
+      <c r="L35" s="12">
+        <f>$K$33/K35</f>
+        <v>3.82540057204743</v>
+      </c>
+      <c r="M35" s="12">
+        <f>L35/D35</f>
+        <v>0.9563501430118575</v>
+      </c>
+      <c r="N35" s="21">
         <f t="shared" si="5"/>
-        <v>0.51211118464592986</v>
+        <v>288088</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="9">
+        <v>4</v>
+      </c>
+      <c r="D36" s="15">
+        <v>6</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="14">
+        <v>51370</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="12">
+        <f t="shared" si="4"/>
+        <v>51370</v>
+      </c>
+      <c r="L36" s="12">
+        <f>$K$33/K36</f>
+        <v>5.3633054311855171</v>
+      </c>
+      <c r="M36" s="12">
+        <f>L36/D36</f>
+        <v>0.89388423853091947</v>
+      </c>
+      <c r="N36" s="21">
+        <f t="shared" si="5"/>
+        <v>308220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="9">
+        <v>5</v>
+      </c>
+      <c r="D37" s="15">
+        <v>8</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="14">
+        <v>38814</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="12">
+        <f t="shared" si="4"/>
+        <v>38814</v>
+      </c>
+      <c r="L37" s="12">
+        <f>$K$33/K37</f>
+        <v>7.0982892770649766</v>
+      </c>
+      <c r="M37" s="12">
+        <f>L37/D37</f>
+        <v>0.88728615963312207</v>
+      </c>
+      <c r="N37" s="21">
+        <f t="shared" si="5"/>
+        <v>310512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="9">
+        <v>6</v>
+      </c>
+      <c r="D38" s="15">
+        <v>10</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="14">
+        <v>30870</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="12">
+        <f t="shared" si="4"/>
+        <v>30870</v>
+      </c>
+      <c r="L38" s="12">
+        <f>$K$33/K38</f>
+        <v>8.9249433106575964</v>
+      </c>
+      <c r="M38" s="12">
+        <f>L38/D38</f>
+        <v>0.89249433106575959</v>
+      </c>
+      <c r="N38" s="21">
+        <f t="shared" si="5"/>
+        <v>308700</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="9">
+        <v>7</v>
+      </c>
+      <c r="D39" s="15">
+        <v>12</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="14">
+        <v>26596</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="12">
+        <f t="shared" si="4"/>
+        <v>26596</v>
+      </c>
+      <c r="L39" s="12">
+        <f>$K$33/K39</f>
+        <v>10.359189351782224</v>
+      </c>
+      <c r="M39" s="12">
+        <f>L39/D39</f>
+        <v>0.86326577931518533</v>
+      </c>
+      <c r="N39" s="21">
+        <f t="shared" si="5"/>
+        <v>319152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="9">
+        <v>8</v>
+      </c>
+      <c r="D40" s="15">
+        <v>14</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="14">
+        <v>24638</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="12">
+        <f t="shared" si="4"/>
+        <v>24638</v>
+      </c>
+      <c r="L40" s="12">
+        <f>$K$33/K40</f>
+        <v>11.182441756636091</v>
+      </c>
+      <c r="M40" s="12">
+        <f>L40/D40</f>
+        <v>0.7987458397597208</v>
+      </c>
+      <c r="N40" s="21">
+        <f t="shared" si="5"/>
+        <v>344932</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C41" s="9">
+        <v>9</v>
+      </c>
+      <c r="D41" s="15">
+        <v>16</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="13">
+        <v>24488</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="12">
+        <f t="shared" si="4"/>
+        <v>24488</v>
+      </c>
+      <c r="L41" s="12">
+        <f>$K$33/K41</f>
+        <v>11.250939235543941</v>
+      </c>
+      <c r="M41" s="12">
+        <f>L41/D41</f>
+        <v>0.70318370222149629</v>
+      </c>
+      <c r="N41" s="21">
+        <f t="shared" si="5"/>
+        <v>391808</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C42" s="9">
+        <v>10</v>
+      </c>
+      <c r="D42" s="15">
+        <v>18</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="13">
+        <v>20537</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="12">
+        <f t="shared" si="4"/>
+        <v>20537</v>
+      </c>
+      <c r="L42" s="12">
+        <f>$K$33/K42</f>
+        <v>13.415445293859863</v>
+      </c>
+      <c r="M42" s="12">
+        <f>L42/D42</f>
+        <v>0.74530251632554789</v>
+      </c>
+      <c r="N42" s="21">
+        <f t="shared" si="5"/>
+        <v>369666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C43" s="9">
+        <v>11</v>
+      </c>
+      <c r="D43" s="15">
+        <v>20</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="13">
+        <v>20022</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="12">
+        <f t="shared" si="4"/>
+        <v>20022</v>
+      </c>
+      <c r="L43" s="12">
+        <f>$K$33/K43</f>
+        <v>13.760513435221256</v>
+      </c>
+      <c r="M43" s="12">
+        <f>L43/D43</f>
+        <v>0.68802567176106277</v>
+      </c>
+      <c r="N43" s="21">
+        <f t="shared" si="5"/>
+        <v>400440</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A32:B32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
add test cases to test plan
</commit_message>
<xml_diff>
--- a/project/fractal-parallel-tasks/test-plan.xlsx
+++ b/project/fractal-parallel-tasks/test-plan.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>#</t>
-  </si>
-  <si>
-    <t>g</t>
   </si>
   <si>
     <t>p</t>
@@ -335,19 +332,10 @@
     </r>
   </si>
   <si>
-    <t>image-small</t>
-  </si>
-  <si>
-    <t>image-big</t>
-  </si>
-  <si>
     <t>Fri May 22 16:03:56 EEST 2020</t>
   </si>
   <si>
     <t>Fri May 22 15:36:13 EEST 2020</t>
-  </si>
-  <si>
-    <t>image-huge</t>
   </si>
   <si>
     <t>Mon May 25 19:02:11 EEST 2020</t>
@@ -363,6 +351,24 @@
   </si>
   <si>
     <t>Cp = p*Tp</t>
+  </si>
+  <si>
+    <t>imageSize : 2560x1920</t>
+  </si>
+  <si>
+    <t>Tue May 26 14:08:18 EEST 2020</t>
+  </si>
+  <si>
+    <t>image-1</t>
+  </si>
+  <si>
+    <t>image-2</t>
+  </si>
+  <si>
+    <t>image-3</t>
+  </si>
+  <si>
+    <t>image-4</t>
   </si>
 </sst>
 </file>
@@ -429,13 +435,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <vertAlign val="subscript"/>
@@ -471,6 +470,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -523,15 +527,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -541,29 +539,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -578,10 +567,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -686,7 +679,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Sp(1)</c:v>
+            <c:v>Sp(640x480)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -702,10 +695,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -738,16 +731,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$7:$L$17</c:f>
+              <c:f>Sheet1!$K$7:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -780,6 +779,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11.209189391109451</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.093171880255634</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.701497860199714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,12 +809,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -842,6 +895,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -852,7 +911,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Sp(2)</c:v>
+            <c:v>Sp(1280x960)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -866,12 +925,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$20:$L$30</c:f>
+              <c:f>Sheet1!$K$22:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -904,6 +1011,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10.242223692918596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.643790849673202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.702164768646764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,7 +1027,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Sp(3)</c:v>
+            <c:v>Sp(1920x1440)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -928,12 +1041,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$33:$L$43</c:f>
+              <c:f>Sheet1!$K$37:$K$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -966,6 +1127,128 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>13.760513435221256</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.96836902800659</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.040800870923462</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Sp(2560x1920)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$52:$K$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9304968233747521</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6998829953198129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4014120594431478</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0570425364140865</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5950241003152978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.162510176972191</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.461555190411753</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.2653340918494</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.23599174014957</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.718727404193782</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.980752792760928</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.363908909212041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,11 +1264,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1193285664"/>
-        <c:axId val="1193286208"/>
+        <c:axId val="161072"/>
+        <c:axId val="161616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1193285664"/>
+        <c:axId val="161072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1372,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1193286208"/>
+        <c:crossAx val="161616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,7 +1380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1193286208"/>
+        <c:axId val="161616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1488,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1193285664"/>
+        <c:crossAx val="161072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1367,7 +1650,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Ep(1)</c:v>
+            <c:v>Ep(640x480)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1383,10 +1666,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$22:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1419,16 +1702,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$7:$M$17</c:f>
+              <c:f>Sheet1!$L$7:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1461,6 +1750,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.56045946955547254</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45878054001161972</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.44589574417498806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,7 +1766,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Ep(2)</c:v>
+            <c:v>Ep(1280x960)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1485,12 +1780,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$20:$M$30</c:f>
+              <c:f>Sheet1!$L$22:$L$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1523,6 +1866,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.51211118464592986</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57471776589423651</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.52925686536028183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,7 +1882,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Ep(3)</c:v>
+            <c:v>Ep(1920x1440)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1547,12 +1896,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$33:$M$43</c:f>
+              <c:f>Sheet1!$L$37:$L$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1585,6 +1982,128 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.68802567176106277</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.58947131945484499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.54336670295514422</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Ep(2560x1920)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$52:$L$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96524841168737607</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92497074882995323</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90023534324052468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88213031705176081</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85950241003152983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8468758480810159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81868251360083943</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76658338074058752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73533287445275386</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68593637020968912</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63548876330731485</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59849620455050168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,11 +2119,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1466140288"/>
-        <c:axId val="1466150080"/>
+        <c:axId val="159984"/>
+        <c:axId val="152368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1466140288"/>
+        <c:axId val="159984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +2227,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1466150080"/>
+        <c:crossAx val="152368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +2235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1466150080"/>
+        <c:axId val="152368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,7 +2342,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1466140288"/>
+        <c:crossAx val="159984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1989,7 +2508,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Cp(1)</c:v>
+            <c:v>Cp(640x480)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2005,10 +2524,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$52:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2041,16 +2560,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$7:$N$17</c:f>
+              <c:f>Sheet1!$M$7:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>30007</c:v>
                 </c:pt>
@@ -2083,6 +2608,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>53540</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65406</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,7 +2624,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Cp(2)</c:v>
+            <c:v>Cp(1280x960)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2109,10 +2640,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$52:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2145,16 +2676,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$20:$N$30</c:f>
+              <c:f>Sheet1!$M$22:$M$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>123808</c:v>
                 </c:pt>
@@ -2187,6 +2724,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>241760</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>215424</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>233928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2197,7 +2740,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Cp(3)</c:v>
+            <c:v>Cp(1920x1440)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2213,10 +2756,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$17</c:f>
+              <c:f>Sheet1!$D$52:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2249,16 +2792,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$33:$N$43</c:f>
+              <c:f>Sheet1!$M$37:$M$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>275513</c:v>
                 </c:pt>
@@ -2291,6 +2840,128 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>400440</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>467390</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>507048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Cp(2560x1920)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$52:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$52:$M$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>474325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>491402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>526890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>537704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>551860</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>560088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>579376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>618752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>645048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>691500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>746394</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>792528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,11 +2977,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1466137024"/>
-        <c:axId val="1466139744"/>
+        <c:axId val="1983813424"/>
+        <c:axId val="1983816688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1466137024"/>
+        <c:axId val="1983813424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,7 +3085,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1466139744"/>
+        <c:crossAx val="1983816688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2422,7 +3093,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1466139744"/>
+        <c:axId val="1983816688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2530,7 +3201,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1466137024"/>
+        <c:crossAx val="1983813424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4283,15 +4954,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>192157</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>168965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>448235</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4313,15 +4984,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>188259</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>174811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>448235</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>13446</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4343,15 +5014,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>197222</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>129989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>510987</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>4483</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4637,10 +5308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:N43"/>
+  <dimension ref="A5:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4648,1273 +5319,2019 @@
     <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="5.21875" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" customWidth="1"/>
-    <col min="7" max="10" width="6.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="14" width="10.88671875" customWidth="1"/>
+    <col min="5" max="6" width="7.77734375" customWidth="1"/>
+    <col min="7" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="12" max="13" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>30250</v>
+      </c>
+      <c r="F7" s="9">
+        <v>30751</v>
+      </c>
+      <c r="G7" s="9">
+        <v>30007</v>
+      </c>
+      <c r="H7" s="9">
+        <v>30526</v>
+      </c>
+      <c r="I7" s="9">
+        <v>31256</v>
+      </c>
+      <c r="J7" s="7">
+        <f>MIN(E7:I7)</f>
+        <v>30007</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
+        <f>D7*J7</f>
+        <v>30007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>15908</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="7">
+        <f t="shared" ref="J8:J17" si="0">MIN(E8:I8)</f>
+        <v>15908</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" ref="K8:K19" si="1">$J$7/J8</f>
+        <v>1.8862836308775459</v>
+      </c>
+      <c r="L8" s="7">
+        <f>K8/D8</f>
+        <v>0.94314181543877296</v>
+      </c>
+      <c r="M8" s="7">
+        <f>D8*J8</f>
+        <v>31816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="6">
         <v>3</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="D9" s="10">
         <v>4</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="14">
-        <v>30250</v>
-      </c>
-      <c r="G7" s="14">
-        <v>30751</v>
-      </c>
-      <c r="H7" s="14">
-        <v>30007</v>
-      </c>
-      <c r="I7" s="14">
-        <v>30526</v>
-      </c>
-      <c r="J7" s="14">
-        <v>31256</v>
-      </c>
-      <c r="K7" s="12">
-        <f>MIN(F7:J7)</f>
-        <v>30007</v>
-      </c>
-      <c r="L7" s="12">
-        <v>1</v>
-      </c>
-      <c r="M7" s="12">
-        <v>1</v>
-      </c>
-      <c r="N7" s="21">
-        <f>D7*K7</f>
-        <v>30007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="15">
-        <v>2</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14">
-        <v>15908</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12">
-        <f t="shared" ref="K8:K17" si="0">MIN(F8:J8)</f>
-        <v>15908</v>
-      </c>
-      <c r="L8" s="12">
-        <f>$K$7/K8</f>
-        <v>1.8862836308775459</v>
-      </c>
-      <c r="M8" s="12">
-        <f>L8/D8</f>
-        <v>0.94314181543877296</v>
-      </c>
-      <c r="N8" s="21">
-        <f t="shared" ref="N8:N17" si="1">D8*K8</f>
-        <v>31816</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="9">
-        <v>3</v>
-      </c>
-      <c r="D9" s="15">
-        <v>4</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="14">
+      <c r="E9" s="9">
         <v>8578</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="7">
         <f t="shared" si="0"/>
         <v>8578</v>
       </c>
-      <c r="L9" s="12">
-        <f>$K$7/K9</f>
+      <c r="K9" s="7">
+        <f t="shared" si="1"/>
         <v>3.4981347633480997</v>
       </c>
-      <c r="M9" s="12">
-        <f>L9/D9</f>
+      <c r="L9" s="7">
+        <f>K9/D9</f>
         <v>0.87453369083702492</v>
       </c>
-      <c r="N9" s="21">
-        <f t="shared" si="1"/>
+      <c r="M9" s="7">
+        <f>D9*J9</f>
         <v>34312</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>4</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>6</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="14">
+      <c r="E10" s="9">
         <v>6086</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
         <v>6086</v>
       </c>
-      <c r="L10" s="12">
-        <f>$K$7/K10</f>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
         <v>4.9304962208347023</v>
       </c>
-      <c r="M10" s="12">
-        <f>L10/D10</f>
+      <c r="L10" s="7">
+        <f>K10/D10</f>
         <v>0.82174937013911709</v>
       </c>
-      <c r="N10" s="21">
-        <f t="shared" si="1"/>
+      <c r="M10" s="7">
+        <f>D10*J10</f>
         <v>36516</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>8</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="14">
+      <c r="E11" s="9">
         <v>4828</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="7">
         <f t="shared" si="0"/>
         <v>4828</v>
       </c>
-      <c r="L11" s="12">
-        <f>$K$7/K11</f>
+      <c r="K11" s="7">
+        <f t="shared" si="1"/>
         <v>6.2152029826014914</v>
       </c>
-      <c r="M11" s="12">
-        <f>L11/D11</f>
+      <c r="L11" s="7">
+        <f>K11/D11</f>
         <v>0.77690037282518642</v>
       </c>
-      <c r="N11" s="21">
-        <f t="shared" si="1"/>
+      <c r="M11" s="7">
+        <f>D11*J11</f>
         <v>38624</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>6</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="14">
+      <c r="E12" s="9">
         <v>3973</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="7">
         <f t="shared" si="0"/>
         <v>3973</v>
       </c>
-      <c r="L12" s="12">
-        <f>$K$7/K12</f>
+      <c r="K12" s="7">
+        <f t="shared" si="1"/>
         <v>7.5527309338031712</v>
       </c>
-      <c r="M12" s="12">
-        <f>L12/D12</f>
+      <c r="L12" s="7">
+        <f>K12/D12</f>
         <v>0.75527309338031712</v>
       </c>
-      <c r="N12" s="21">
-        <f t="shared" si="1"/>
+      <c r="M12" s="7">
+        <f>D12*J12</f>
         <v>39730</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="9">
+      <c r="C13" s="6">
         <v>7</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>12</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="14">
+      <c r="E13" s="9">
         <v>3482</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="7">
         <f t="shared" si="0"/>
         <v>3482</v>
       </c>
-      <c r="L13" s="12">
-        <f>$K$7/K13</f>
+      <c r="K13" s="7">
+        <f t="shared" si="1"/>
         <v>8.6177484204480184</v>
       </c>
-      <c r="M13" s="12">
-        <f>L13/D13</f>
+      <c r="L13" s="7">
+        <f>K13/D13</f>
         <v>0.71814570170400149</v>
       </c>
-      <c r="N13" s="21">
-        <f t="shared" si="1"/>
+      <c r="M13" s="7">
+        <f>D13*J13</f>
         <v>41784</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <v>8</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="10">
         <v>14</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="14">
+      <c r="E14" s="9">
         <v>3268</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="7">
         <f t="shared" si="0"/>
         <v>3268</v>
       </c>
-      <c r="L14" s="12">
-        <f>$K$7/K14</f>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
         <v>9.1820685434516527</v>
       </c>
-      <c r="M14" s="12">
-        <f>L14/D14</f>
+      <c r="L14" s="7">
+        <f>K14/D14</f>
         <v>0.65586203881797522</v>
       </c>
-      <c r="N14" s="21">
-        <f t="shared" si="1"/>
+      <c r="M14" s="7">
+        <f>D14*J14</f>
         <v>45752</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="9">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="6">
         <v>9</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="10">
         <v>16</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13">
+      <c r="E15" s="8">
         <v>2997</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="12">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="7">
         <f t="shared" si="0"/>
         <v>2997</v>
       </c>
-      <c r="L15" s="12">
-        <f>$K$7/K15</f>
+      <c r="K15" s="7">
+        <f t="shared" si="1"/>
         <v>10.012345679012345</v>
       </c>
-      <c r="M15" s="12">
-        <f>L15/D15</f>
+      <c r="L15" s="7">
+        <f>K15/D15</f>
         <v>0.62577160493827155</v>
       </c>
-      <c r="N15" s="21">
-        <f t="shared" si="1"/>
+      <c r="M15" s="7">
+        <f>D15*J15</f>
         <v>47952</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="9">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="6">
         <v>10</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="10">
         <v>18</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13">
+      <c r="E16" s="8">
         <v>2849</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="12">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="7">
         <f t="shared" si="0"/>
         <v>2849</v>
       </c>
-      <c r="L16" s="12">
-        <f>$K$7/K16</f>
+      <c r="K16" s="7">
+        <f t="shared" si="1"/>
         <v>10.532467532467532</v>
       </c>
-      <c r="M16" s="12">
-        <f>L16/D16</f>
+      <c r="L16" s="7">
+        <f>K16/D16</f>
         <v>0.58513708513708507</v>
       </c>
-      <c r="N16" s="21">
-        <f t="shared" si="1"/>
+      <c r="M16" s="7">
+        <f>D16*J16</f>
         <v>51282</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="9">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="6">
         <v>11</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="10">
         <v>20</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13">
+      <c r="E17" s="8">
         <v>2677</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="12">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="7">
         <f t="shared" si="0"/>
         <v>2677</v>
       </c>
-      <c r="L17" s="12">
-        <f>$K$7/K17</f>
+      <c r="K17" s="7">
+        <f t="shared" si="1"/>
         <v>11.209189391109451</v>
       </c>
-      <c r="M17" s="12">
-        <f>L17/D17</f>
+      <c r="L17" s="7">
+        <f>K17/D17</f>
         <v>0.56045946955547254</v>
       </c>
-      <c r="N17" s="21">
+      <c r="M17" s="7">
+        <f>D17*J17</f>
+        <v>53540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="6">
+        <v>12</v>
+      </c>
+      <c r="D18" s="10">
+        <v>22</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2973</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3026</v>
+      </c>
+      <c r="G18" s="8">
+        <v>3044</v>
+      </c>
+      <c r="H18" s="8">
+        <v>3046</v>
+      </c>
+      <c r="I18" s="8">
+        <v>3112</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" ref="J18" si="2">MIN(E18:I18)</f>
+        <v>2973</v>
+      </c>
+      <c r="K18" s="7">
         <f t="shared" si="1"/>
-        <v>53540</v>
+        <v>10.093171880255634</v>
+      </c>
+      <c r="L18" s="7">
+        <f>K18/D18</f>
+        <v>0.45878054001161972</v>
+      </c>
+      <c r="M18" s="7">
+        <f>D18*J18</f>
+        <v>65406</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D18" s="4"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="6">
+        <v>13</v>
+      </c>
+      <c r="D19" s="10">
+        <v>24</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2942</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2849</v>
+      </c>
+      <c r="G19" s="8">
+        <v>3140</v>
+      </c>
+      <c r="H19" s="8">
+        <v>2804</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2942</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" ref="J19" si="3">MIN(E19:I19)</f>
+        <v>2804</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="1"/>
+        <v>10.701497860199714</v>
+      </c>
+      <c r="L19" s="7">
+        <f>K19/D19</f>
+        <v>0.44589574417498806</v>
+      </c>
+      <c r="M19" s="7">
+        <f>D19*J19</f>
+        <v>67296</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>123808</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="7">
+        <f>MIN(E22:I22)</f>
+        <v>123808</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1</v>
+      </c>
+      <c r="M22" s="7">
+        <f>D22*J22</f>
+        <v>123808</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="6">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>64728</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="7">
+        <f t="shared" ref="J23:J32" si="4">MIN(E23:I23)</f>
+        <v>64728</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" ref="K23:K34" si="5">$J$22/J23</f>
+        <v>1.9127425534544555</v>
+      </c>
+      <c r="L23" s="7">
+        <f>K23/D23</f>
+        <v>0.95637127672722777</v>
+      </c>
+      <c r="M23" s="7">
+        <f>D23*J23</f>
+        <v>129456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="6">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
+        <v>4</v>
+      </c>
+      <c r="E24" s="9">
+        <v>33076</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="7">
+        <f t="shared" si="4"/>
+        <v>33076</v>
+      </c>
+      <c r="K24" s="7">
+        <f t="shared" si="5"/>
+        <v>3.7431370177772405</v>
+      </c>
+      <c r="L24" s="7">
+        <f>K24/D24</f>
+        <v>0.93578425444431013</v>
+      </c>
+      <c r="M24" s="7">
+        <f>D24*J24</f>
+        <v>132304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25" s="10">
+        <v>6</v>
+      </c>
+      <c r="E25" s="9">
+        <v>22862</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="7">
+        <f t="shared" si="4"/>
+        <v>22862</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="5"/>
+        <v>5.4154492170413784</v>
+      </c>
+      <c r="L25" s="7">
+        <f>K25/D25</f>
+        <v>0.90257486950689636</v>
+      </c>
+      <c r="M25" s="7">
+        <f>D25*J25</f>
+        <v>137172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+      <c r="D26" s="10">
+        <v>8</v>
+      </c>
+      <c r="E26" s="9">
+        <v>17802</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="7">
+        <f t="shared" si="4"/>
+        <v>17802</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="5"/>
+        <v>6.9547241882934498</v>
+      </c>
+      <c r="L26" s="7">
+        <f>K26/D26</f>
+        <v>0.86934052353668123</v>
+      </c>
+      <c r="M26" s="7">
+        <f>D26*J26</f>
+        <v>142416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="6">
+        <v>6</v>
+      </c>
+      <c r="D27" s="10">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9">
+        <v>14251</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="7">
+        <f t="shared" si="4"/>
+        <v>14251</v>
+      </c>
+      <c r="K27" s="7">
+        <f t="shared" si="5"/>
+        <v>8.687671040628727</v>
+      </c>
+      <c r="L27" s="7">
+        <f>K27/D27</f>
+        <v>0.86876710406287272</v>
+      </c>
+      <c r="M27" s="7">
+        <f>D27*J27</f>
+        <v>142510</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="6">
+        <v>7</v>
+      </c>
+      <c r="D28" s="10">
         <v>12</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="5" t="s">
+      <c r="E28" s="9">
+        <v>13104</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="7">
+        <f t="shared" si="4"/>
+        <v>13104</v>
+      </c>
+      <c r="K28" s="7">
+        <f t="shared" si="5"/>
+        <v>9.4481074481074483</v>
+      </c>
+      <c r="L28" s="7">
+        <f>K28/D28</f>
+        <v>0.78734228734228739</v>
+      </c>
+      <c r="M28" s="7">
+        <f>D28*J28</f>
+        <v>157248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="6">
+        <v>8</v>
+      </c>
+      <c r="D29" s="10">
+        <v>14</v>
+      </c>
+      <c r="E29" s="9">
+        <v>12141</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="7">
+        <f t="shared" si="4"/>
+        <v>12141</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="5"/>
+        <v>10.197512560744585</v>
+      </c>
+      <c r="L29" s="7">
+        <f>K29/D29</f>
+        <v>0.72839375433889886</v>
+      </c>
+      <c r="M29" s="7">
+        <f>D29*J29</f>
+        <v>169974</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="6">
+        <v>9</v>
+      </c>
+      <c r="D30" s="10">
+        <v>16</v>
+      </c>
+      <c r="E30" s="8">
+        <v>11002</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="7">
+        <f t="shared" si="4"/>
+        <v>11002</v>
+      </c>
+      <c r="K30" s="7">
+        <f t="shared" si="5"/>
+        <v>11.253226686057081</v>
+      </c>
+      <c r="L30" s="7">
+        <f>K30/D30</f>
+        <v>0.70332666787856757</v>
+      </c>
+      <c r="M30" s="7">
+        <f>D30*J30</f>
+        <v>176032</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C31" s="6">
+        <v>10</v>
+      </c>
+      <c r="D31" s="10">
+        <v>18</v>
+      </c>
+      <c r="E31" s="8">
+        <v>11093</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="7">
+        <f t="shared" si="4"/>
+        <v>11093</v>
+      </c>
+      <c r="K31" s="7">
+        <f t="shared" si="5"/>
+        <v>11.160912287027855</v>
+      </c>
+      <c r="L31" s="7">
+        <f>K31/D31</f>
+        <v>0.62005068261265861</v>
+      </c>
+      <c r="M31" s="7">
+        <f>D31*J31</f>
+        <v>199674</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C32" s="6">
+        <v>11</v>
+      </c>
+      <c r="D32" s="10">
+        <v>20</v>
+      </c>
+      <c r="E32" s="8">
+        <v>12088</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="7">
+        <f t="shared" si="4"/>
+        <v>12088</v>
+      </c>
+      <c r="K32" s="7">
+        <f t="shared" si="5"/>
+        <v>10.242223692918596</v>
+      </c>
+      <c r="L32" s="7">
+        <f>K32/D32</f>
+        <v>0.51211118464592986</v>
+      </c>
+      <c r="M32" s="7">
+        <f>D32*J32</f>
+        <v>241760</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C33" s="6">
+        <v>12</v>
+      </c>
+      <c r="D33" s="10">
+        <v>22</v>
+      </c>
+      <c r="E33" s="8">
+        <v>10428</v>
+      </c>
+      <c r="F33" s="8">
+        <v>10164</v>
+      </c>
+      <c r="G33" s="8">
+        <v>9792</v>
+      </c>
+      <c r="H33" s="8">
+        <v>9944</v>
+      </c>
+      <c r="I33" s="8">
+        <v>9963</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" ref="J33:J34" si="6">MIN(E33:I33)</f>
+        <v>9792</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="5"/>
+        <v>12.643790849673202</v>
+      </c>
+      <c r="L33" s="7">
+        <f>K33/D33</f>
+        <v>0.57471776589423651</v>
+      </c>
+      <c r="M33" s="7">
+        <f>D33*J33</f>
+        <v>215424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C34" s="6">
+        <v>13</v>
+      </c>
+      <c r="D34" s="10">
+        <v>24</v>
+      </c>
+      <c r="E34" s="8">
+        <v>9747</v>
+      </c>
+      <c r="F34" s="8">
+        <v>10155</v>
+      </c>
+      <c r="G34" s="8">
+        <v>9956</v>
+      </c>
+      <c r="H34" s="8">
+        <v>10126</v>
+      </c>
+      <c r="I34" s="8">
+        <v>9754</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="6"/>
+        <v>9747</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="5"/>
+        <v>12.702164768646764</v>
+      </c>
+      <c r="L34" s="7">
+        <f>K34/D34</f>
+        <v>0.52925686536028183</v>
+      </c>
+      <c r="M34" s="7">
+        <f>D34*J34</f>
+        <v>233928</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="9">
+        <v>275513</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="7">
+        <f>MIN(E37:I37)</f>
+        <v>275513</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1</v>
+      </c>
+      <c r="L37" s="7">
+        <v>1</v>
+      </c>
+      <c r="M37" s="7">
+        <f>D37*J37</f>
+        <v>275513</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="6">
+        <v>2</v>
+      </c>
+      <c r="D38" s="10">
+        <v>2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>142684</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="7">
+        <f t="shared" ref="J38:J49" si="7">MIN(E38:I38)</f>
+        <v>142684</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" ref="K38:K49" si="8">$J$37/J38</f>
+        <v>1.930931288721931</v>
+      </c>
+      <c r="L38" s="7">
+        <f>K38/D38</f>
+        <v>0.96546564436096549</v>
+      </c>
+      <c r="M38" s="7">
+        <f>D38*J38</f>
+        <v>285368</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="6">
         <v>3</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="D39" s="10">
         <v>4</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="E39" s="9">
+        <v>72022</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="7">
+        <f t="shared" si="7"/>
+        <v>72022</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="8"/>
+        <v>3.82540057204743</v>
+      </c>
+      <c r="L39" s="7">
+        <f>K39/D39</f>
+        <v>0.9563501430118575</v>
+      </c>
+      <c r="M39" s="7">
+        <f>D39*J39</f>
+        <v>288088</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="6">
+        <v>4</v>
+      </c>
+      <c r="D40" s="10">
+        <v>6</v>
+      </c>
+      <c r="E40" s="9">
+        <v>51370</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="7">
+        <f t="shared" si="7"/>
+        <v>51370</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="8"/>
+        <v>5.3633054311855171</v>
+      </c>
+      <c r="L40" s="7">
+        <f>K40/D40</f>
+        <v>0.89388423853091947</v>
+      </c>
+      <c r="M40" s="7">
+        <f>D40*J40</f>
+        <v>308220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="6">
         <v>5</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="D41" s="10">
+        <v>8</v>
+      </c>
+      <c r="E41" s="9">
+        <v>38814</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="7">
+        <f t="shared" si="7"/>
+        <v>38814</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="8"/>
+        <v>7.0982892770649766</v>
+      </c>
+      <c r="L41" s="7">
+        <f>K41/D41</f>
+        <v>0.88728615963312207</v>
+      </c>
+      <c r="M41" s="7">
+        <f>D41*J41</f>
+        <v>310512</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="6">
         <v>6</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="D42" s="10">
+        <v>10</v>
+      </c>
+      <c r="E42" s="9">
+        <v>30870</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="7">
+        <f t="shared" si="7"/>
+        <v>30870</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="8"/>
+        <v>8.9249433106575964</v>
+      </c>
+      <c r="L42" s="7">
+        <f>K42/D42</f>
+        <v>0.89249433106575959</v>
+      </c>
+      <c r="M42" s="7">
+        <f>D42*J42</f>
+        <v>308700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="6">
         <v>7</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="D43" s="10">
+        <v>12</v>
+      </c>
+      <c r="E43" s="9">
+        <v>26596</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="7">
+        <f t="shared" si="7"/>
+        <v>26596</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="8"/>
+        <v>10.359189351782224</v>
+      </c>
+      <c r="L43" s="7">
+        <f>K43/D43</f>
+        <v>0.86326577931518533</v>
+      </c>
+      <c r="M43" s="7">
+        <f>D43*J43</f>
+        <v>319152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="6">
         <v>8</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="D44" s="10">
+        <v>14</v>
+      </c>
+      <c r="E44" s="9">
+        <v>24638</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="7">
+        <f t="shared" si="7"/>
+        <v>24638</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="8"/>
+        <v>11.182441756636091</v>
+      </c>
+      <c r="L44" s="7">
+        <f>K44/D44</f>
+        <v>0.7987458397597208</v>
+      </c>
+      <c r="M44" s="7">
+        <f>D44*J44</f>
+        <v>344932</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C45" s="6">
         <v>9</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="D45" s="10">
+        <v>16</v>
+      </c>
+      <c r="E45" s="8">
+        <v>24488</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="7">
+        <f t="shared" si="7"/>
+        <v>24488</v>
+      </c>
+      <c r="K45" s="7">
+        <f t="shared" si="8"/>
+        <v>11.250939235543941</v>
+      </c>
+      <c r="L45" s="7">
+        <f>K45/D45</f>
+        <v>0.70318370222149629</v>
+      </c>
+      <c r="M45" s="7">
+        <f>D45*J45</f>
+        <v>391808</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C46" s="6">
         <v>10</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="D46" s="10">
+        <v>18</v>
+      </c>
+      <c r="E46" s="8">
+        <v>20537</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="7">
+        <f t="shared" si="7"/>
+        <v>20537</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" si="8"/>
+        <v>13.415445293859863</v>
+      </c>
+      <c r="L46" s="7">
+        <f>K46/D46</f>
+        <v>0.74530251632554789</v>
+      </c>
+      <c r="M46" s="7">
+        <f>D46*J46</f>
+        <v>369666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C47" s="6">
+        <v>11</v>
+      </c>
+      <c r="D47" s="10">
         <v>20</v>
       </c>
+      <c r="E47" s="8">
+        <v>20022</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="7">
+        <f t="shared" si="7"/>
+        <v>20022</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="8"/>
+        <v>13.760513435221256</v>
+      </c>
+      <c r="L47" s="7">
+        <f>K47/D47</f>
+        <v>0.68802567176106277</v>
+      </c>
+      <c r="M47" s="7">
+        <f>D47*J47</f>
+        <v>400440</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C48" s="6">
+        <v>12</v>
+      </c>
+      <c r="D48" s="10">
+        <v>22</v>
+      </c>
+      <c r="E48" s="8">
+        <v>21325</v>
+      </c>
+      <c r="F48" s="8">
+        <v>21459</v>
+      </c>
+      <c r="G48" s="8">
+        <v>21277</v>
+      </c>
+      <c r="H48" s="8">
+        <v>21245</v>
+      </c>
+      <c r="I48" s="8">
+        <v>21338</v>
+      </c>
+      <c r="J48" s="7">
+        <f t="shared" si="7"/>
+        <v>21245</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" si="8"/>
+        <v>12.96836902800659</v>
+      </c>
+      <c r="L48" s="7">
+        <f>K48/D48</f>
+        <v>0.58947131945484499</v>
+      </c>
+      <c r="M48" s="7">
+        <f>D48*J48</f>
+        <v>467390</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C49" s="6">
         <v>13</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="9">
+      <c r="D49" s="10">
+        <v>24</v>
+      </c>
+      <c r="E49" s="8">
+        <v>21170</v>
+      </c>
+      <c r="F49" s="8">
+        <v>21135</v>
+      </c>
+      <c r="G49" s="8">
+        <v>21214</v>
+      </c>
+      <c r="H49" s="8">
+        <v>21127</v>
+      </c>
+      <c r="I49" s="8">
+        <v>21222</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" si="7"/>
+        <v>21127</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="8"/>
+        <v>13.040800870923462</v>
+      </c>
+      <c r="L49" s="7">
+        <f>K49/D49</f>
+        <v>0.54336670295514422</v>
+      </c>
+      <c r="M49" s="7">
+        <f>D49*J49</f>
+        <v>507048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="15">
+      <c r="E51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="6">
         <v>1</v>
       </c>
-      <c r="E20" s="10">
+      <c r="D52" s="10">
+        <v>1</v>
+      </c>
+      <c r="E52" s="9">
+        <v>484061</v>
+      </c>
+      <c r="F52" s="9">
+        <v>475600</v>
+      </c>
+      <c r="G52" s="9">
+        <v>475107</v>
+      </c>
+      <c r="H52" s="9">
+        <v>475168</v>
+      </c>
+      <c r="I52" s="9">
+        <v>474325</v>
+      </c>
+      <c r="J52" s="7">
+        <f>MIN(E52:I52)</f>
+        <v>474325</v>
+      </c>
+      <c r="K52" s="7">
+        <v>1</v>
+      </c>
+      <c r="L52" s="7">
+        <v>1</v>
+      </c>
+      <c r="M52" s="7">
+        <f>D52*J52</f>
+        <v>474325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="6">
         <v>2</v>
       </c>
-      <c r="F20" s="14">
-        <v>123808</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12">
-        <f>MIN(F20:J20)</f>
-        <v>123808</v>
-      </c>
-      <c r="L20" s="12">
-        <v>1</v>
-      </c>
-      <c r="M20" s="12">
-        <v>1</v>
-      </c>
-      <c r="N20" s="21">
-        <f>D20*K20</f>
-        <v>123808</v>
+      <c r="D53" s="10">
+        <v>2</v>
+      </c>
+      <c r="E53" s="9">
+        <v>245701</v>
+      </c>
+      <c r="F53" s="17">
+        <v>271714</v>
+      </c>
+      <c r="G53" s="17">
+        <v>274180</v>
+      </c>
+      <c r="H53" s="17">
+        <v>248261</v>
+      </c>
+      <c r="I53" s="17">
+        <v>287478</v>
+      </c>
+      <c r="J53" s="7">
+        <f t="shared" ref="J53:J64" si="9">MIN(E53:I53)</f>
+        <v>245701</v>
+      </c>
+      <c r="K53" s="7">
+        <f>$J$52/J53</f>
+        <v>1.9304968233747521</v>
+      </c>
+      <c r="L53" s="7">
+        <f>K53/D53</f>
+        <v>0.96524841168737607</v>
+      </c>
+      <c r="M53" s="7">
+        <f>D53*J53</f>
+        <v>491402</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+      <c r="C54" s="6">
+        <v>3</v>
+      </c>
+      <c r="D54" s="10">
+        <v>4</v>
+      </c>
+      <c r="E54" s="9">
+        <v>128200</v>
+      </c>
+      <c r="F54" s="17">
+        <v>129910</v>
+      </c>
+      <c r="G54" s="17">
+        <v>133203</v>
+      </c>
+      <c r="H54" s="17">
+        <v>129504</v>
+      </c>
+      <c r="I54" s="17">
+        <v>129624</v>
+      </c>
+      <c r="J54" s="7">
+        <f t="shared" si="9"/>
+        <v>128200</v>
+      </c>
+      <c r="K54" s="7">
+        <f t="shared" ref="K54:K64" si="10">$J$52/J54</f>
+        <v>3.6998829953198129</v>
+      </c>
+      <c r="L54" s="7">
+        <f>K54/D54</f>
+        <v>0.92497074882995323</v>
+      </c>
+      <c r="M54" s="7">
+        <f>D54*J54</f>
+        <v>512800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+      <c r="C55" s="6">
+        <v>4</v>
+      </c>
+      <c r="D55" s="10">
+        <v>6</v>
+      </c>
+      <c r="E55" s="9">
+        <v>87815</v>
+      </c>
+      <c r="F55" s="17">
+        <v>88337</v>
+      </c>
+      <c r="G55" s="17">
+        <v>89009</v>
+      </c>
+      <c r="H55" s="17">
+        <v>89828</v>
+      </c>
+      <c r="I55" s="17">
+        <v>89186</v>
+      </c>
+      <c r="J55" s="7">
+        <f t="shared" si="9"/>
+        <v>87815</v>
+      </c>
+      <c r="K55" s="7">
+        <f t="shared" si="10"/>
+        <v>5.4014120594431478</v>
+      </c>
+      <c r="L55" s="7">
+        <f>K55/D55</f>
+        <v>0.90023534324052468</v>
+      </c>
+      <c r="M55" s="7">
+        <f>D55*J55</f>
+        <v>526890</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+      <c r="C56" s="6">
+        <v>5</v>
+      </c>
+      <c r="D56" s="10">
+        <v>8</v>
+      </c>
+      <c r="E56" s="9">
+        <v>67649</v>
+      </c>
+      <c r="F56" s="17">
+        <v>67213</v>
+      </c>
+      <c r="G56" s="17">
+        <v>67950</v>
+      </c>
+      <c r="H56" s="17">
+        <v>67932</v>
+      </c>
+      <c r="I56" s="17">
+        <v>67936</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" si="9"/>
+        <v>67213</v>
+      </c>
+      <c r="K56" s="7">
+        <f t="shared" si="10"/>
+        <v>7.0570425364140865</v>
+      </c>
+      <c r="L56" s="7">
+        <f>K56/D56</f>
+        <v>0.88213031705176081</v>
+      </c>
+      <c r="M56" s="7">
+        <f>D56*J56</f>
+        <v>537704</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+      <c r="C57" s="6">
+        <v>6</v>
+      </c>
+      <c r="D57" s="10">
+        <v>10</v>
+      </c>
+      <c r="E57" s="9">
+        <v>55227</v>
+      </c>
+      <c r="F57" s="17">
+        <v>55558</v>
+      </c>
+      <c r="G57" s="17">
+        <v>55186</v>
+      </c>
+      <c r="H57" s="17">
+        <v>56226</v>
+      </c>
+      <c r="I57" s="17">
+        <v>55670</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="9"/>
+        <v>55186</v>
+      </c>
+      <c r="K57" s="7">
+        <f t="shared" si="10"/>
+        <v>8.5950241003152978</v>
+      </c>
+      <c r="L57" s="7">
+        <f>K57/D57</f>
+        <v>0.85950241003152983</v>
+      </c>
+      <c r="M57" s="7">
+        <f>D57*J57</f>
+        <v>551860</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+      <c r="C58" s="6">
+        <v>7</v>
+      </c>
+      <c r="D58" s="10">
+        <v>12</v>
+      </c>
+      <c r="E58" s="9">
+        <v>47248</v>
+      </c>
+      <c r="F58" s="17">
+        <v>46674</v>
+      </c>
+      <c r="G58" s="17">
+        <v>46743</v>
+      </c>
+      <c r="H58" s="17">
+        <v>46735</v>
+      </c>
+      <c r="I58" s="17">
+        <v>46728</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" si="9"/>
+        <v>46674</v>
+      </c>
+      <c r="K58" s="7">
+        <f t="shared" si="10"/>
+        <v>10.162510176972191</v>
+      </c>
+      <c r="L58" s="7">
+        <f>K58/D58</f>
+        <v>0.8468758480810159</v>
+      </c>
+      <c r="M58" s="7">
+        <f>D58*J58</f>
+        <v>560088</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+      <c r="C59" s="6">
+        <v>8</v>
+      </c>
+      <c r="D59" s="10">
+        <v>14</v>
+      </c>
+      <c r="E59" s="9">
+        <v>43142</v>
+      </c>
+      <c r="F59" s="17">
+        <v>41749</v>
+      </c>
+      <c r="G59" s="17">
+        <v>41384</v>
+      </c>
+      <c r="H59" s="17">
+        <v>43296</v>
+      </c>
+      <c r="I59" s="17">
+        <v>42551</v>
+      </c>
+      <c r="J59" s="7">
+        <f t="shared" si="9"/>
+        <v>41384</v>
+      </c>
+      <c r="K59" s="7">
+        <f t="shared" si="10"/>
+        <v>11.461555190411753</v>
+      </c>
+      <c r="L59" s="7">
+        <f>K59/D59</f>
+        <v>0.81868251360083943</v>
+      </c>
+      <c r="M59" s="7">
+        <f>D59*J59</f>
+        <v>579376</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C60" s="6">
+        <v>9</v>
+      </c>
+      <c r="D60" s="10">
+        <v>16</v>
+      </c>
+      <c r="E60" s="8">
+        <v>39933</v>
+      </c>
+      <c r="F60" s="17">
+        <v>39848</v>
+      </c>
+      <c r="G60" s="17">
+        <v>40740</v>
+      </c>
+      <c r="H60" s="17">
+        <v>38672</v>
+      </c>
+      <c r="I60" s="17">
+        <v>38895</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="9"/>
+        <v>38672</v>
+      </c>
+      <c r="K60" s="7">
+        <f t="shared" si="10"/>
+        <v>12.2653340918494</v>
+      </c>
+      <c r="L60" s="7">
+        <f>K60/D60</f>
+        <v>0.76658338074058752</v>
+      </c>
+      <c r="M60" s="7">
+        <f>D60*J60</f>
+        <v>618752</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C61" s="6">
+        <v>10</v>
+      </c>
+      <c r="D61" s="10">
         <v>18</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="9">
-        <v>2</v>
-      </c>
-      <c r="D21" s="15">
-        <v>2</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="14">
-        <v>64728</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12">
-        <f t="shared" ref="K21:K30" si="2">MIN(F21:J21)</f>
-        <v>64728</v>
-      </c>
-      <c r="L21" s="12">
-        <f>$K$20/K21</f>
-        <v>1.9127425534544555</v>
-      </c>
-      <c r="M21" s="12">
-        <f>L21/D21</f>
-        <v>0.95637127672722777</v>
-      </c>
-      <c r="N21" s="21">
-        <f t="shared" ref="N21:N30" si="3">D21*K21</f>
-        <v>129456</v>
+      <c r="E61" s="8">
+        <v>36670</v>
+      </c>
+      <c r="F61" s="17">
+        <v>36997</v>
+      </c>
+      <c r="G61" s="17">
+        <v>35839</v>
+      </c>
+      <c r="H61" s="17">
+        <v>36378</v>
+      </c>
+      <c r="I61" s="17">
+        <v>35836</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="9"/>
+        <v>35836</v>
+      </c>
+      <c r="K61" s="7">
+        <f t="shared" si="10"/>
+        <v>13.23599174014957</v>
+      </c>
+      <c r="L61" s="7">
+        <f>K61/D61</f>
+        <v>0.73533287445275386</v>
+      </c>
+      <c r="M61" s="7">
+        <f>D61*J61</f>
+        <v>645048</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="9">
-        <v>3</v>
-      </c>
-      <c r="D22" s="15">
-        <v>4</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="14">
-        <v>33076</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12">
-        <f t="shared" si="2"/>
-        <v>33076</v>
-      </c>
-      <c r="L22" s="12">
-        <f>$K$20/K22</f>
-        <v>3.7431370177772405</v>
-      </c>
-      <c r="M22" s="12">
-        <f>L22/D22</f>
-        <v>0.93578425444431013</v>
-      </c>
-      <c r="N22" s="21">
-        <f t="shared" si="3"/>
-        <v>132304</v>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C62" s="6">
+        <v>11</v>
+      </c>
+      <c r="D62" s="10">
+        <v>20</v>
+      </c>
+      <c r="E62" s="8">
+        <v>34575</v>
+      </c>
+      <c r="F62" s="17">
+        <v>34915</v>
+      </c>
+      <c r="G62" s="17">
+        <v>34626</v>
+      </c>
+      <c r="H62" s="17">
+        <v>34836</v>
+      </c>
+      <c r="I62" s="17">
+        <v>34814</v>
+      </c>
+      <c r="J62" s="18">
+        <f t="shared" si="9"/>
+        <v>34575</v>
+      </c>
+      <c r="K62" s="18">
+        <f t="shared" si="10"/>
+        <v>13.718727404193782</v>
+      </c>
+      <c r="L62" s="18">
+        <f>K62/D62</f>
+        <v>0.68593637020968912</v>
+      </c>
+      <c r="M62" s="18">
+        <f>D62*J62</f>
+        <v>691500</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="15">
-        <v>6</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="14">
-        <v>22862</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12">
-        <f t="shared" si="2"/>
-        <v>22862</v>
-      </c>
-      <c r="L23" s="12">
-        <f>$K$20/K23</f>
-        <v>5.4154492170413784</v>
-      </c>
-      <c r="M23" s="12">
-        <f>L23/D23</f>
-        <v>0.90257486950689636</v>
-      </c>
-      <c r="N23" s="21">
-        <f t="shared" si="3"/>
-        <v>137172</v>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C63" s="6">
+        <v>12</v>
+      </c>
+      <c r="D63" s="10">
+        <v>22</v>
+      </c>
+      <c r="E63" s="17">
+        <v>34738</v>
+      </c>
+      <c r="F63" s="17">
+        <v>34075</v>
+      </c>
+      <c r="G63" s="17">
+        <v>34004</v>
+      </c>
+      <c r="H63" s="17">
+        <v>34087</v>
+      </c>
+      <c r="I63" s="17">
+        <v>33927</v>
+      </c>
+      <c r="J63" s="18">
+        <f t="shared" si="9"/>
+        <v>33927</v>
+      </c>
+      <c r="K63" s="18">
+        <f t="shared" si="10"/>
+        <v>13.980752792760928</v>
+      </c>
+      <c r="L63" s="18">
+        <f t="shared" ref="L63:L64" si="11">K63/D63</f>
+        <v>0.63548876330731485</v>
+      </c>
+      <c r="M63" s="18">
+        <f t="shared" ref="M63:M64" si="12">D63*J63</f>
+        <v>746394</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="9">
-        <v>5</v>
-      </c>
-      <c r="D24" s="15">
-        <v>8</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="14">
-        <v>17802</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="12">
-        <f t="shared" si="2"/>
-        <v>17802</v>
-      </c>
-      <c r="L24" s="12">
-        <f>$K$20/K24</f>
-        <v>6.9547241882934498</v>
-      </c>
-      <c r="M24" s="12">
-        <f>L24/D24</f>
-        <v>0.86934052353668123</v>
-      </c>
-      <c r="N24" s="21">
-        <f t="shared" si="3"/>
-        <v>142416</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
-      <c r="C25" s="9">
-        <v>6</v>
-      </c>
-      <c r="D25" s="15">
-        <v>10</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="14">
-        <v>14251</v>
-      </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="12">
-        <f t="shared" si="2"/>
-        <v>14251</v>
-      </c>
-      <c r="L25" s="12">
-        <f>$K$20/K25</f>
-        <v>8.687671040628727</v>
-      </c>
-      <c r="M25" s="12">
-        <f>L25/D25</f>
-        <v>0.86876710406287272</v>
-      </c>
-      <c r="N25" s="21">
-        <f t="shared" si="3"/>
-        <v>142510</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="9">
-        <v>7</v>
-      </c>
-      <c r="D26" s="15">
-        <v>12</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="14">
-        <v>13104</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="12">
-        <f t="shared" si="2"/>
-        <v>13104</v>
-      </c>
-      <c r="L26" s="12">
-        <f>$K$20/K26</f>
-        <v>9.4481074481074483</v>
-      </c>
-      <c r="M26" s="12">
-        <f>L26/D26</f>
-        <v>0.78734228734228739</v>
-      </c>
-      <c r="N26" s="21">
-        <f t="shared" si="3"/>
-        <v>157248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="C27" s="9">
-        <v>8</v>
-      </c>
-      <c r="D27" s="15">
-        <v>14</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="14">
-        <v>12141</v>
-      </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="12">
-        <f t="shared" si="2"/>
-        <v>12141</v>
-      </c>
-      <c r="L27" s="12">
-        <f>$K$20/K27</f>
-        <v>10.197512560744585</v>
-      </c>
-      <c r="M27" s="12">
-        <f>L27/D27</f>
-        <v>0.72839375433889886</v>
-      </c>
-      <c r="N27" s="21">
-        <f t="shared" si="3"/>
-        <v>169974</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C28" s="9">
-        <v>9</v>
-      </c>
-      <c r="D28" s="15">
-        <v>16</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="13">
-        <v>11002</v>
-      </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="12">
-        <f t="shared" si="2"/>
-        <v>11002</v>
-      </c>
-      <c r="L28" s="12">
-        <f>$K$20/K28</f>
-        <v>11.253226686057081</v>
-      </c>
-      <c r="M28" s="12">
-        <f>L28/D28</f>
-        <v>0.70332666787856757</v>
-      </c>
-      <c r="N28" s="21">
-        <f t="shared" si="3"/>
-        <v>176032</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C29" s="9">
-        <v>10</v>
-      </c>
-      <c r="D29" s="15">
-        <v>18</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="13">
-        <v>11093</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="12">
-        <f t="shared" si="2"/>
-        <v>11093</v>
-      </c>
-      <c r="L29" s="12">
-        <f>$K$20/K29</f>
-        <v>11.160912287027855</v>
-      </c>
-      <c r="M29" s="12">
-        <f>L29/D29</f>
-        <v>0.62005068261265861</v>
-      </c>
-      <c r="N29" s="21">
-        <f t="shared" si="3"/>
-        <v>199674</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C30" s="9">
-        <v>11</v>
-      </c>
-      <c r="D30" s="15">
-        <v>20</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="13">
-        <v>12088</v>
-      </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="12">
-        <f t="shared" si="2"/>
-        <v>12088</v>
-      </c>
-      <c r="L30" s="12">
-        <f>$K$20/K30</f>
-        <v>10.242223692918596</v>
-      </c>
-      <c r="M30" s="12">
-        <f>L30/D30</f>
-        <v>0.51211118464592986</v>
-      </c>
-      <c r="N30" s="21">
-        <f t="shared" si="3"/>
-        <v>241760</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N32" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="15">
-        <v>1</v>
-      </c>
-      <c r="E33" s="10">
-        <v>2</v>
-      </c>
-      <c r="F33" s="14">
-        <v>275513</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="12">
-        <f>MIN(F33:J33)</f>
-        <v>275513</v>
-      </c>
-      <c r="L33" s="12">
-        <v>1</v>
-      </c>
-      <c r="M33" s="12">
-        <v>1</v>
-      </c>
-      <c r="N33" s="21">
-        <f>D33*K33</f>
-        <v>275513</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="9">
-        <v>2</v>
-      </c>
-      <c r="D34" s="15">
-        <v>2</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="14">
-        <v>142684</v>
-      </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="12">
-        <f t="shared" ref="K34:K43" si="4">MIN(F34:J34)</f>
-        <v>142684</v>
-      </c>
-      <c r="L34" s="12">
-        <f>$K$33/K34</f>
-        <v>1.930931288721931</v>
-      </c>
-      <c r="M34" s="12">
-        <f>L34/D34</f>
-        <v>0.96546564436096549</v>
-      </c>
-      <c r="N34" s="21">
-        <f t="shared" ref="N34:N43" si="5">D34*K34</f>
-        <v>285368</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="9">
-        <v>3</v>
-      </c>
-      <c r="D35" s="15">
-        <v>4</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="14">
-        <v>72022</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="12">
-        <f t="shared" si="4"/>
-        <v>72022</v>
-      </c>
-      <c r="L35" s="12">
-        <f>$K$33/K35</f>
-        <v>3.82540057204743</v>
-      </c>
-      <c r="M35" s="12">
-        <f>L35/D35</f>
-        <v>0.9563501430118575</v>
-      </c>
-      <c r="N35" s="21">
-        <f t="shared" si="5"/>
-        <v>288088</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="9">
-        <v>4</v>
-      </c>
-      <c r="D36" s="15">
-        <v>6</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="14">
-        <v>51370</v>
-      </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="12">
-        <f t="shared" si="4"/>
-        <v>51370</v>
-      </c>
-      <c r="L36" s="12">
-        <f>$K$33/K36</f>
-        <v>5.3633054311855171</v>
-      </c>
-      <c r="M36" s="12">
-        <f>L36/D36</f>
-        <v>0.89388423853091947</v>
-      </c>
-      <c r="N36" s="21">
-        <f t="shared" si="5"/>
-        <v>308220</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B37" s="1"/>
-      <c r="C37" s="9">
-        <v>5</v>
-      </c>
-      <c r="D37" s="15">
-        <v>8</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="14">
-        <v>38814</v>
-      </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="12">
-        <f t="shared" si="4"/>
-        <v>38814</v>
-      </c>
-      <c r="L37" s="12">
-        <f>$K$33/K37</f>
-        <v>7.0982892770649766</v>
-      </c>
-      <c r="M37" s="12">
-        <f>L37/D37</f>
-        <v>0.88728615963312207</v>
-      </c>
-      <c r="N37" s="21">
-        <f t="shared" si="5"/>
-        <v>310512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
-      <c r="C38" s="9">
-        <v>6</v>
-      </c>
-      <c r="D38" s="15">
-        <v>10</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="14">
-        <v>30870</v>
-      </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="12">
-        <f t="shared" si="4"/>
-        <v>30870</v>
-      </c>
-      <c r="L38" s="12">
-        <f>$K$33/K38</f>
-        <v>8.9249433106575964</v>
-      </c>
-      <c r="M38" s="12">
-        <f>L38/D38</f>
-        <v>0.89249433106575959</v>
-      </c>
-      <c r="N38" s="21">
-        <f t="shared" si="5"/>
-        <v>308700</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B39" s="1"/>
-      <c r="C39" s="9">
-        <v>7</v>
-      </c>
-      <c r="D39" s="15">
-        <v>12</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="14">
-        <v>26596</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="12">
-        <f t="shared" si="4"/>
-        <v>26596</v>
-      </c>
-      <c r="L39" s="12">
-        <f>$K$33/K39</f>
-        <v>10.359189351782224</v>
-      </c>
-      <c r="M39" s="12">
-        <f>L39/D39</f>
-        <v>0.86326577931518533</v>
-      </c>
-      <c r="N39" s="21">
-        <f t="shared" si="5"/>
-        <v>319152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-      <c r="C40" s="9">
-        <v>8</v>
-      </c>
-      <c r="D40" s="15">
-        <v>14</v>
-      </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="14">
-        <v>24638</v>
-      </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="12">
-        <f t="shared" si="4"/>
-        <v>24638</v>
-      </c>
-      <c r="L40" s="12">
-        <f>$K$33/K40</f>
-        <v>11.182441756636091</v>
-      </c>
-      <c r="M40" s="12">
-        <f>L40/D40</f>
-        <v>0.7987458397597208</v>
-      </c>
-      <c r="N40" s="21">
-        <f t="shared" si="5"/>
-        <v>344932</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C41" s="9">
-        <v>9</v>
-      </c>
-      <c r="D41" s="15">
-        <v>16</v>
-      </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="13">
-        <v>24488</v>
-      </c>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="12">
-        <f t="shared" si="4"/>
-        <v>24488</v>
-      </c>
-      <c r="L41" s="12">
-        <f>$K$33/K41</f>
-        <v>11.250939235543941</v>
-      </c>
-      <c r="M41" s="12">
-        <f>L41/D41</f>
-        <v>0.70318370222149629</v>
-      </c>
-      <c r="N41" s="21">
-        <f t="shared" si="5"/>
-        <v>391808</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C42" s="9">
-        <v>10</v>
-      </c>
-      <c r="D42" s="15">
-        <v>18</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="13">
-        <v>20537</v>
-      </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="12">
-        <f t="shared" si="4"/>
-        <v>20537</v>
-      </c>
-      <c r="L42" s="12">
-        <f>$K$33/K42</f>
-        <v>13.415445293859863</v>
-      </c>
-      <c r="M42" s="12">
-        <f>L42/D42</f>
-        <v>0.74530251632554789</v>
-      </c>
-      <c r="N42" s="21">
-        <f t="shared" si="5"/>
-        <v>369666</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C43" s="9">
-        <v>11</v>
-      </c>
-      <c r="D43" s="15">
-        <v>20</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="13">
-        <v>20022</v>
-      </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="12">
-        <f t="shared" si="4"/>
-        <v>20022</v>
-      </c>
-      <c r="L43" s="12">
-        <f>$K$33/K43</f>
-        <v>13.760513435221256</v>
-      </c>
-      <c r="M43" s="12">
-        <f>L43/D43</f>
-        <v>0.68802567176106277</v>
-      </c>
-      <c r="N43" s="21">
-        <f t="shared" si="5"/>
-        <v>400440</v>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C64" s="6">
+        <v>13</v>
+      </c>
+      <c r="D64" s="10">
+        <v>24</v>
+      </c>
+      <c r="E64" s="17">
+        <v>33247</v>
+      </c>
+      <c r="F64" s="17">
+        <v>33056</v>
+      </c>
+      <c r="G64" s="17">
+        <v>33046</v>
+      </c>
+      <c r="H64" s="17">
+        <v>33022</v>
+      </c>
+      <c r="I64" s="17">
+        <v>33202</v>
+      </c>
+      <c r="J64" s="18">
+        <f t="shared" si="9"/>
+        <v>33022</v>
+      </c>
+      <c r="K64" s="18">
+        <f t="shared" si="10"/>
+        <v>14.363908909212041</v>
+      </c>
+      <c r="L64" s="18">
+        <f t="shared" si="11"/>
+        <v>0.59849620455050168</v>
+      </c>
+      <c r="M64" s="18">
+        <f t="shared" si="12"/>
+        <v>792528</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A33:B33"/>
+  <mergeCells count="12">
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change sync, add rectangles to test plan
</commit_message>
<xml_diff>
--- a/project/fractal-parallel-tasks/test-plan.xlsx
+++ b/project/fractal-parallel-tasks/test-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14772" windowHeight="8844"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14772" windowHeight="8844" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="image" sheetId="1" r:id="rId1"/>
@@ -1294,11 +1294,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302307088"/>
-        <c:axId val="302300016"/>
+        <c:axId val="659526256"/>
+        <c:axId val="659530064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302307088"/>
+        <c:axId val="659526256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1402,7 +1402,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302300016"/>
+        <c:crossAx val="659530064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1410,7 +1410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302300016"/>
+        <c:axId val="659530064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1518,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302307088"/>
+        <c:crossAx val="659526256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2149,11 +2149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302306000"/>
-        <c:axId val="302307632"/>
+        <c:axId val="659532784"/>
+        <c:axId val="659531696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302306000"/>
+        <c:axId val="659532784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2257,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302307632"/>
+        <c:crossAx val="659531696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2265,7 +2265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302307632"/>
+        <c:axId val="659531696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2372,7 +2372,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302306000"/>
+        <c:crossAx val="659532784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3007,11 +3007,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302308176"/>
-        <c:axId val="302300560"/>
+        <c:axId val="659527888"/>
+        <c:axId val="659529520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302308176"/>
+        <c:axId val="659527888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3115,7 +3115,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302300560"/>
+        <c:crossAx val="659529520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3123,7 +3123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302300560"/>
+        <c:axId val="659529520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3231,7 +3231,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302308176"/>
+        <c:crossAx val="659527888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3866,11 +3866,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302302192"/>
-        <c:axId val="271127136"/>
+        <c:axId val="659538224"/>
+        <c:axId val="659528976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302302192"/>
+        <c:axId val="659538224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3974,7 +3974,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271127136"/>
+        <c:crossAx val="659528976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3982,7 +3982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="271127136"/>
+        <c:axId val="659528976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4090,7 +4090,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302302192"/>
+        <c:crossAx val="659538224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4605,11 +4605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="271121152"/>
-        <c:axId val="472896880"/>
+        <c:axId val="659532240"/>
+        <c:axId val="659531152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="271121152"/>
+        <c:axId val="659532240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4713,7 +4713,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472896880"/>
+        <c:crossAx val="659531152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4721,7 +4721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472896880"/>
+        <c:axId val="659531152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4828,7 +4828,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271121152"/>
+        <c:crossAx val="659532240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5347,11 +5347,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="472886544"/>
-        <c:axId val="472899056"/>
+        <c:axId val="659533872"/>
+        <c:axId val="659534960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472886544"/>
+        <c:axId val="659533872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5455,7 +5455,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472899056"/>
+        <c:crossAx val="659534960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5463,7 +5463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472899056"/>
+        <c:axId val="659534960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5571,7 +5571,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472886544"/>
+        <c:crossAx val="659533872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9394,430 +9394,6 @@
           <cell r="K7">
             <v>1</v>
           </cell>
-          <cell r="L7">
-            <v>1</v>
-          </cell>
-          <cell r="M7">
-            <v>133414</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="K8">
-            <v>2.1534711797653059</v>
-          </cell>
-          <cell r="L8">
-            <v>1.0767355898826529</v>
-          </cell>
-          <cell r="M8">
-            <v>123906</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="K9">
-            <v>4.0400327044786968</v>
-          </cell>
-          <cell r="L9">
-            <v>1.0100081761196742</v>
-          </cell>
-          <cell r="M9">
-            <v>132092</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="K10">
-            <v>5.8697698974877905</v>
-          </cell>
-          <cell r="L10">
-            <v>0.97829498291463179</v>
-          </cell>
-          <cell r="M10">
-            <v>136374</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="K11">
-            <v>7.5764665795899822</v>
-          </cell>
-          <cell r="L11">
-            <v>0.94705832244874777</v>
-          </cell>
-          <cell r="M11">
-            <v>140872</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="K12">
-            <v>9.2174934365068406</v>
-          </cell>
-          <cell r="L12">
-            <v>0.92174934365068406</v>
-          </cell>
-          <cell r="M12">
-            <v>144740</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="K13">
-            <v>10.58085494488064</v>
-          </cell>
-          <cell r="L13">
-            <v>0.8817379120733867</v>
-          </cell>
-          <cell r="M13">
-            <v>151308</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="K14">
-            <v>11.866405763586231</v>
-          </cell>
-          <cell r="L14">
-            <v>0.84760041168473077</v>
-          </cell>
-          <cell r="M14">
-            <v>157402</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="K15">
-            <v>12.368035598405488</v>
-          </cell>
-          <cell r="L15">
-            <v>0.77300222490034298</v>
-          </cell>
-          <cell r="M15">
-            <v>172592</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="K16">
-            <v>12.768111781031678</v>
-          </cell>
-          <cell r="L16">
-            <v>0.70933954339064875</v>
-          </cell>
-          <cell r="M16">
-            <v>188082</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="K17">
-            <v>13.306802313983642</v>
-          </cell>
-          <cell r="L17">
-            <v>0.66534011569918206</v>
-          </cell>
-          <cell r="M17">
-            <v>200520</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="K18">
-            <v>13.825284974093265</v>
-          </cell>
-          <cell r="L18">
-            <v>0.62842204427696657</v>
-          </cell>
-          <cell r="M18">
-            <v>212300</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="K19">
-            <v>14.150827322868052</v>
-          </cell>
-          <cell r="L19">
-            <v>0.58961780511950213</v>
-          </cell>
-          <cell r="M19">
-            <v>226272</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="K22">
-            <v>1</v>
-          </cell>
-          <cell r="L22">
-            <v>1</v>
-          </cell>
-          <cell r="M22">
-            <v>132022</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="K23">
-            <v>1.9154443235400798</v>
-          </cell>
-          <cell r="L23">
-            <v>0.95772216177003988</v>
-          </cell>
-          <cell r="M23">
-            <v>137850</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="K24">
-            <v>3.3034405104466407</v>
-          </cell>
-          <cell r="L24">
-            <v>0.82586012761166017</v>
-          </cell>
-          <cell r="M24">
-            <v>159860</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="K25">
-            <v>5.0818738211632475</v>
-          </cell>
-          <cell r="L25">
-            <v>0.84697897019387458</v>
-          </cell>
-          <cell r="M25">
-            <v>155874</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="K26">
-            <v>6.3704883227176223</v>
-          </cell>
-          <cell r="L26">
-            <v>0.79631104033970279</v>
-          </cell>
-          <cell r="M26">
-            <v>165792</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="K27">
-            <v>7.9244897959183671</v>
-          </cell>
-          <cell r="L27">
-            <v>0.79244897959183669</v>
-          </cell>
-          <cell r="M27">
-            <v>166600</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="K28">
-            <v>8.8534066523605155</v>
-          </cell>
-          <cell r="L28">
-            <v>0.73778388769670966</v>
-          </cell>
-          <cell r="M28">
-            <v>178944</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="K29">
-            <v>8.8202832709780861</v>
-          </cell>
-          <cell r="L29">
-            <v>0.63002023364129189</v>
-          </cell>
-          <cell r="M29">
-            <v>209552</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="K30">
-            <v>9.4072965654838256</v>
-          </cell>
-          <cell r="L30">
-            <v>0.5879560353427391</v>
-          </cell>
-          <cell r="M30">
-            <v>224544</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="K31">
-            <v>9.9242276178305637</v>
-          </cell>
-          <cell r="L31">
-            <v>0.55134597876836466</v>
-          </cell>
-          <cell r="M31">
-            <v>239454</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="K32">
-            <v>10.211307912444891</v>
-          </cell>
-          <cell r="L32">
-            <v>0.51056539562224457</v>
-          </cell>
-          <cell r="M32">
-            <v>258580</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="K33">
-            <v>10.482096069868996</v>
-          </cell>
-          <cell r="L33">
-            <v>0.47645891226677256</v>
-          </cell>
-          <cell r="M33">
-            <v>277090</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="K34">
-            <v>10.479599936497857</v>
-          </cell>
-          <cell r="L34">
-            <v>0.43664999735407739</v>
-          </cell>
-          <cell r="M34">
-            <v>302352</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="K37">
-            <v>1</v>
-          </cell>
-          <cell r="L37">
-            <v>1</v>
-          </cell>
-          <cell r="M37">
-            <v>114396</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="K38">
-            <v>1.9480944109533054</v>
-          </cell>
-          <cell r="L38">
-            <v>0.97404720547665269</v>
-          </cell>
-          <cell r="M38">
-            <v>117444</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="K39">
-            <v>3.5879936016058713</v>
-          </cell>
-          <cell r="L39">
-            <v>0.89699840040146783</v>
-          </cell>
-          <cell r="M39">
-            <v>127532</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="K40">
-            <v>5.3393698949824975</v>
-          </cell>
-          <cell r="L40">
-            <v>0.88989498249708288</v>
-          </cell>
-          <cell r="M40">
-            <v>128550</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="K41">
-            <v>6.6874780778674152</v>
-          </cell>
-          <cell r="L41">
-            <v>0.8359347597334269</v>
-          </cell>
-          <cell r="M41">
-            <v>136848</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="K42">
-            <v>8.1160695282014892</v>
-          </cell>
-          <cell r="L42">
-            <v>0.81160695282014894</v>
-          </cell>
-          <cell r="M42">
-            <v>140950</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="K43">
-            <v>9.2187928116689495</v>
-          </cell>
-          <cell r="L43">
-            <v>0.76823273430574579</v>
-          </cell>
-          <cell r="M43">
-            <v>148908</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="K44">
-            <v>10.361018023729734</v>
-          </cell>
-          <cell r="L44">
-            <v>0.74007271598069535</v>
-          </cell>
-          <cell r="M44">
-            <v>154574</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="K45">
-            <v>10.276320517427237</v>
-          </cell>
-          <cell r="L45">
-            <v>0.64227003233920232</v>
-          </cell>
-          <cell r="M45">
-            <v>178112</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="K46">
-            <v>11.229606361048395</v>
-          </cell>
-          <cell r="L46">
-            <v>0.62386702005824413</v>
-          </cell>
-          <cell r="M46">
-            <v>183366</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="K47">
-            <v>11.63506916192026</v>
-          </cell>
-          <cell r="L47">
-            <v>0.58175345809601298</v>
-          </cell>
-          <cell r="M47">
-            <v>196640</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="K48">
-            <v>12.119504184765335</v>
-          </cell>
-          <cell r="L48">
-            <v>0.55088655385296981</v>
-          </cell>
-          <cell r="M48">
-            <v>207658</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="K49">
-            <v>12.532427695004381</v>
-          </cell>
-          <cell r="L49">
-            <v>0.52218448729184919</v>
-          </cell>
-          <cell r="M49">
-            <v>219072</v>
-          </cell>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -10090,13 +9666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="5.21875" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" customWidth="1"/>
     <col min="5" max="6" width="7.77734375" customWidth="1"/>
@@ -12123,8 +11699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M62"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N57" sqref="N57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>